<commit_message>
Final code commit, resolved bugs
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLOHOKA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay_lohokare/Desktop/excelUploadAutomation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908BDAAA-22F8-5847-AACE-CE604E9A8EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>fileName</t>
   </si>
@@ -80,113 +81,32 @@
     <t>UPLOAD_TIME</t>
   </si>
   <si>
-    <t>ICIS Monthly.xlsx</t>
-  </si>
-  <si>
-    <t>Upload Template</t>
-  </si>
-  <si>
-    <t>A, C:G</t>
-  </si>
-  <si>
-    <t>EXCEL_UPLOAD_ICIS_INDEX_TEST</t>
-  </si>
-  <si>
-    <t>Metric Name,  MONTH</t>
-  </si>
-  <si>
-    <t>MONTH, VALUE, Metric Name, REGION, PRODUCT, CURR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Metric Name: str, MONTH:str, VALUE: float,  UPLOAD_TIME:datetime64[ns]</t>
-  </si>
-  <si>
-    <t>Customer Master_Updated.xlsx</t>
-  </si>
-  <si>
-    <t>Sheet1</t>
-  </si>
-  <si>
-    <t>A:AD</t>
-  </si>
-  <si>
     <t>ignore</t>
   </si>
   <si>
-    <t>EXCEL_UPLOAD_MACH1_SHIPTO_TST3</t>
-  </si>
-  <si>
-    <t>Cust/Sales Area: str
-,Sales Organization: str
-,BU: str
-,Shipto ID: str
-,Soldto ID: str
-,Soldto Name: str
-,Parent ID: str
-,Parent Name: str
-,Sales Manager ID: str
-,Sales Manager: str
-,Sales Person ID: str
-,Sales Person Name: str
-,Cust.Serv.Cl.of Sold to: str
-,Cust.Serv.Cl.ShipTo: str
-,Cust Class Name: str
-,Alt Cust Grp3: str
-,Alt Cust Grp2: str
-,Alt Cust Grp1: str
-,AREA: str
-,Area Name: str
-,REGION: str
-,Region Name: str
-,SUPERREGION: str
-,SuperRegion Name: str
-,Ship to Country ID: str
-,Ship to Country Name: str
-,VOLUME: str
-,LOCATION: str
-,Country Sub Div: str
-,Country Sub Div Code: str
-,UPLOAD_TIME: str</t>
-  </si>
-  <si>
-    <t>Cust/Sales Area
-,Sales Organization
-,BU
-,Shipto ID
-,Soldto ID
-,Soldto Name
-,Parent ID
-,Parent Name
-,Sales Manager ID
-,Sales Manager
-,Sales Person ID
-,Sales Person Name
-,Cust.Serv.Cl.of Sold to
-,Cust.Serv.Cl.ShipTo
-,Cust Class Name
-,Alt Cust Grp3
-,Alt Cust Grp2
-,Alt Cust Grp1
-,AREA
-,Area Name
-,REGION
-,Region Name
-,SUPERREGION
-,SuperRegion Name
-,Ship to Country ID
-,Ship to Country Name
-,VOLUME
-,LOCATION
-,Country Sub Div
-,Country Sub Div Code</t>
+    <t>DP_ZEMA_IHS_DAILY.xls</t>
+  </si>
+  <si>
+    <t>Zema_Export</t>
+  </si>
+  <si>
+    <t>A:J</t>
+  </si>
+  <si>
+    <t>Date: IHS Daily, Product: PRODUCT, Concept: CONCEPT, Geography: GEOGRAPHY, Grade: GRADE, Terms: TERMS, Unit: UNIT, Price: PRICE</t>
+  </si>
+  <si>
+    <t>DP_ZEMA_IHS_DAILY_BKUP</t>
+  </si>
+  <si>
+    <t>UPLOAD_TIME: datetime64, IHS Daily: datetime64, PRICE: float, Price ID: float, PRODUCT : str, Product Code: str, GEOGRAPHY:str, CONCEPT:str, GRADE: str, TERMS:str, Price ID:float, UNIT: str</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,34 +129,44 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF44546A"/>
       <name val="EMprint"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -244,33 +174,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -581,37 +583,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" style="5"/>
+    <col min="2" max="2" width="10.6640625" style="2"/>
     <col min="3" max="3" width="39.83203125" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.25" customWidth="1"/>
-    <col min="9" max="9" width="28.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="42.9140625" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="65.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="52" customWidth="1"/>
     <col min="11" max="11" width="27.6640625" customWidth="1"/>
     <col min="12" max="13" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" customWidth="1"/>
-    <col min="15" max="15" width="20.08203125" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
     <col min="16" max="16" width="21.33203125" customWidth="1"/>
-    <col min="17" max="17" width="17.08203125" customWidth="1"/>
-    <col min="18" max="18" width="51.25" style="4" customWidth="1"/>
-    <col min="19" max="19" width="23.9140625" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="76.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="18" thickBot="1">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>28</v>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -631,7 +633,7 @@
       <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" t="s">
@@ -658,109 +660,49 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:20" ht="52" thickBot="1">
+      <c r="A2" s="3">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="2"/>
-      <c r="Q2" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" s="5"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>